<commit_message>
fixed bias problem in random phase, fixed upsample method poor performance
</commit_message>
<xml_diff>
--- a/config/jspecs - one carrier.xlsx
+++ b/config/jspecs - one carrier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\p3388_general_rfi_tv\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BB28BD-9995-4AD0-A6D5-448C7FE861CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD7B44B-0425-4C41-A396-DB0509B8BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O183"/>
+  <dimension ref="A1:O182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -563,9 +563,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1976,14 +1974,6 @@
       <c r="J182" s="2"/>
       <c r="M182" s="2"/>
     </row>
-    <row r="183" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D183" s="2"/>
-      <c r="E183" s="2"/>
-      <c r="F183" s="2"/>
-      <c r="G183" s="2"/>
-      <c r="J183" s="2"/>
-      <c r="M183" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>